<commit_message>
feat: Added company_id primary key and foreign key relationship between company data and student data, updated upload function
</commit_message>
<xml_diff>
--- a/excel_files_to_upload/student_data.xlsx
+++ b/excel_files_to_upload/student_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bf09d77fea5249cc/NP/Year 3.2/DevOps/testing/Flask4Python/uploaded_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bf09d77fea5249cc/NP/Year 3.2/DevOps/Git Projects/DevOps_Oct2022_Team4_Assignment/excel_files_to_upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{052B822A-BB87-4F82-8153-8B67F3E75A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F55A58E-5456-4965-9C16-584D6C77DEB0}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{052B822A-BB87-4F82-8153-8B67F3E75A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1D6FF29-64C6-4977-891A-546D1B6C5FC6}"/>
   <bookViews>
-    <workbookView xWindow="10890" yWindow="4020" windowWidth="17415" windowHeight="9675" xr2:uid="{A13D96F5-40AA-4A95-81D3-1E5055213CF6}"/>
+    <workbookView minimized="1" xWindow="15780" yWindow="8265" windowWidth="11400" windowHeight="6990" xr2:uid="{A13D96F5-40AA-4A95-81D3-1E5055213CF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>Student_ID</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>S2206960D</t>
+  </si>
+  <si>
+    <t>Company_ID</t>
   </si>
 </sst>
 </file>
@@ -464,7 +467,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -472,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80D27E27-B554-42B4-B583-D66F690DF968}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E5" sqref="E2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,9 +487,10 @@
     <col min="2" max="2" width="40.7109375" customWidth="1"/>
     <col min="3" max="3" width="56.7109375" customWidth="1"/>
     <col min="4" max="4" width="25.140625" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -499,8 +503,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -514,7 +521,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -528,7 +535,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -542,7 +549,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -556,7 +563,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -570,7 +577,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -584,7 +591,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -598,7 +605,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Modify table to display company list and student status columns
</commit_message>
<xml_diff>
--- a/excel_files_to_upload/student_data.xlsx
+++ b/excel_files_to_upload/student_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bf09d77fea5249cc/NP/Year 3.2/DevOps/Git Projects/DevOps_Oct2022_Team4_Assignment/excel_files_to_upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="8_{052B822A-BB87-4F82-8153-8B67F3E75A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1D6FF29-64C6-4977-891A-546D1B6C5FC6}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="8_{052B822A-BB87-4F82-8153-8B67F3E75A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36DBADB7-48A7-477C-8371-F85C8629B661}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="15780" yWindow="8265" windowWidth="11400" windowHeight="6990" xr2:uid="{A13D96F5-40AA-4A95-81D3-1E5055213CF6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{A13D96F5-40AA-4A95-81D3-1E5055213CF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -172,10 +172,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -478,7 +474,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E2:E5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>